<commit_message>
bug address opco ok
</commit_message>
<xml_diff>
--- a/django_vue/apep/data/BaseOPCO.xlsx
+++ b/django_vue/apep/data/BaseOPCO.xlsx
@@ -1655,10 +1655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G341"/>
+  <dimension ref="A1:F341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A197" workbookViewId="0">
-      <selection activeCell="F322" sqref="F322:F341"/>
+    <sheetView tabSelected="1" topLeftCell="A234" workbookViewId="0">
+      <selection activeCell="F234" sqref="F234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5995,7 +5995,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="225" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="3" t="s">
         <v>247</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="226" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="3" t="s">
         <v>248</v>
       </c>
@@ -6033,7 +6033,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="227" spans="1:7" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:6" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="3" t="s">
         <v>249</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="228" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:6" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="3" t="s">
         <v>250</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="229" spans="1:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A229" s="3" t="s">
         <v>251</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="230" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="3" t="s">
         <v>252</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="231" spans="1:7" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>253</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="232" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="3" t="s">
         <v>254</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="233" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="3" t="s">
         <v>255</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="234" spans="1:7" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A234" s="5" t="s">
         <v>256</v>
       </c>
@@ -6183,7 +6183,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="235" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="3" t="s">
         <v>260</v>
       </c>
@@ -6199,11 +6199,11 @@
       <c r="E235" t="s">
         <v>273</v>
       </c>
-      <c r="G235" t="s">
+      <c r="F235" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="236" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="3" t="s">
         <v>262</v>
       </c>
@@ -6219,11 +6219,11 @@
       <c r="E236" t="s">
         <v>273</v>
       </c>
-      <c r="G236" t="s">
+      <c r="F236" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="237" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="3" t="s">
         <v>263</v>
       </c>
@@ -6239,11 +6239,11 @@
       <c r="E237" t="s">
         <v>273</v>
       </c>
-      <c r="G237" t="s">
+      <c r="F237" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="238" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="3" t="s">
         <v>264</v>
       </c>
@@ -6259,11 +6259,11 @@
       <c r="E238" t="s">
         <v>273</v>
       </c>
-      <c r="G238" t="s">
+      <c r="F238" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="239" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="3" t="s">
         <v>265</v>
       </c>
@@ -6279,11 +6279,11 @@
       <c r="E239" t="s">
         <v>273</v>
       </c>
-      <c r="G239" t="s">
+      <c r="F239" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="240" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="3" t="s">
         <v>267</v>
       </c>
@@ -6299,11 +6299,11 @@
       <c r="E240" t="s">
         <v>273</v>
       </c>
-      <c r="G240" t="s">
+      <c r="F240" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="241" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="3" t="s">
         <v>269</v>
       </c>
@@ -6319,11 +6319,11 @@
       <c r="E241" t="s">
         <v>273</v>
       </c>
-      <c r="G241" t="s">
+      <c r="F241" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="242" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="3" t="s">
         <v>271</v>
       </c>
@@ -6339,11 +6339,11 @@
       <c r="E242" t="s">
         <v>273</v>
       </c>
-      <c r="G242" t="s">
+      <c r="F242" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="243" spans="1:7" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:6" ht="100.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="4" t="s">
         <v>272</v>
       </c>
@@ -6359,11 +6359,11 @@
       <c r="E243" t="s">
         <v>273</v>
       </c>
-      <c r="G243" t="s">
+      <c r="F243" s="7" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="244" spans="1:7" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:6" ht="285.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="3" t="s">
         <v>275</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="245" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="3" t="s">
         <v>276</v>
       </c>
@@ -6403,7 +6403,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="246" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="3" t="s">
         <v>277</v>
       </c>
@@ -6423,7 +6423,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="247" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="3" t="s">
         <v>278</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="248" spans="1:7" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:6" ht="300.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="3" t="s">
         <v>279</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="249" spans="1:7" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:6" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="3" t="s">
         <v>280</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="250" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="3" t="s">
         <v>282</v>
       </c>
@@ -6503,7 +6503,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="251" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A251" s="3" t="s">
         <v>283</v>
       </c>
@@ -6523,7 +6523,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="252" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A252" s="3" t="s">
         <v>284</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="253" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A253" s="3" t="s">
         <v>285</v>
       </c>
@@ -6563,7 +6563,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="254" spans="1:7" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:6" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="3" t="s">
         <v>286</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="255" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A255" s="3" t="s">
         <v>287</v>
       </c>
@@ -6603,7 +6603,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="256" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:6" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A256" s="3" t="s">
         <v>288</v>
       </c>

</xml_diff>